<commit_message>
Corecciones a tests fallando exitosamente!
</commit_message>
<xml_diff>
--- a/series_tiempo_ar_api/apps/validator/tests/samples/catalog.xlsx
+++ b/series_tiempo_ar_api/apps/validator/tests/samples/catalog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="catalog" sheetId="1" state="visible" r:id="rId2"/>
@@ -254,7 +254,7 @@
     <t xml:space="preserve">Evolución de la superficie implantada de viñedos existentes en la República Argentina desde el año 2012 a la última actualización. La información se encuentra en hectáreas y desagregada por provincia.</t>
   </si>
   <si>
-    <t xml:space="preserve">http://datos.agroindustria.gob.ar/dataset/5f97a0b9-f677-4657-9e07-0cd3b98da754/resource/221859a8-c51e-47c2-95ab-a8525bb2b55d/download/serie-tiempo-inv-superficie-de-vinedos-por-pcia-2012-2017.csv</t>
+    <t xml:space="preserve">http://localhost:3456/series_tiempo_ar_api/apps/validator/tests/samples/distribution_missing_column.csv</t>
   </si>
   <si>
     <t xml:space="preserve">serie-tiempo-inv-superficie-de-vinedos-por-pcia-2012-2017.csv</t>
@@ -6276,12 +6276,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -6293,14 +6293,11 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6390,7 +6387,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6405,14 +6402,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="46.4030612244898"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="46.4140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6523,7 +6517,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6538,14 +6532,13 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="29.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="0" width="29.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6598,7 +6591,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>47</v>
       </c>
@@ -6640,9 +6633,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="http://localhost:3456/series_tiempo_ar_api/apps/validator/tests/samples/distribution_missing_column.csv"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6657,14 +6653,11 @@
   </sheetPr>
   <dimension ref="A1:K2535"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -66486,7 +66479,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -66501,14 +66494,11 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -66524,7 +66514,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>